<commit_message>
MaJ divers docs & asm
</commit_message>
<xml_diff>
--- a/DOCS/adressage.xlsx
+++ b/DOCS/adressage.xlsx
@@ -578,8 +578,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -598,163 +602,151 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,20 +758,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1112,7 +1120,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1125,446 +1133,446 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="57"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="53"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="31" t="s">
+      <c r="J2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="51" t="s">
+      <c r="P2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="52"/>
+      <c r="R2" s="50"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="25">
-        <v>0</v>
-      </c>
-      <c r="D3" s="25">
-        <v>0</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="34">
-        <v>0</v>
-      </c>
-      <c r="K3" s="43">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="16">
+        <v>0</v>
+      </c>
+      <c r="K3" s="40">
+        <v>0</v>
+      </c>
+      <c r="L3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="44" t="s">
+      <c r="R3" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="7">
         <v>31</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="33">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="34">
-        <v>1</v>
-      </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="44"/>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="16">
+        <v>1</v>
+      </c>
+      <c r="K4" s="40"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="7">
         <v>32</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="7">
         <v>20</v>
       </c>
-      <c r="E5" s="33">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="34">
-        <v>0</v>
-      </c>
-      <c r="K5" s="43">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0</v>
+      </c>
+      <c r="K5" s="40">
+        <v>1</v>
+      </c>
+      <c r="L5" s="41">
+        <v>0</v>
+      </c>
+      <c r="M5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="44" t="s">
+      <c r="P5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="44"/>
+      <c r="R5" s="25"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="7">
         <v>47</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="33">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="34">
-        <v>1</v>
-      </c>
-      <c r="K6" s="43"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="44"/>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="7">
         <v>48</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="7">
         <v>30</v>
       </c>
-      <c r="E7" s="33">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="34">
-        <v>0</v>
-      </c>
-      <c r="K7" s="43">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0</v>
+      </c>
+      <c r="K7" s="40">
+        <v>1</v>
+      </c>
+      <c r="L7" s="41">
+        <v>1</v>
+      </c>
+      <c r="M7" s="41">
+        <v>0</v>
+      </c>
+      <c r="N7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="43" t="s">
+      <c r="Q7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="R7" s="44"/>
+      <c r="R7" s="25"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="7">
         <v>55</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="7">
         <v>37</v>
       </c>
-      <c r="E8" s="33">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="34">
-        <v>1</v>
-      </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="44"/>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="16">
+        <v>1</v>
+      </c>
+      <c r="K8" s="40"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="25"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="26">
+      <c r="B9" s="37"/>
+      <c r="C9" s="8">
         <v>56</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="8">
         <v>38</v>
       </c>
-      <c r="E9" s="35">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="36">
-        <v>0</v>
-      </c>
-      <c r="K9" s="35">
-        <v>1</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="53" t="s">
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="54"/>
+      <c r="R9" s="57"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="9">
         <v>57</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="9">
         <v>39</v>
       </c>
-      <c r="E10" s="37">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="19">
-        <v>1</v>
-      </c>
-      <c r="K10" s="37">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="37" t="s">
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="R10" s="45" t="s">
+      <c r="R10" s="48" t="s">
         <v>20</v>
       </c>
       <c r="S10" t="s">
@@ -1572,191 +1580,220 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="46"/>
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="9">
         <v>58</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="37">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0</v>
-      </c>
-      <c r="K11" s="18">
-        <v>1</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1</v>
-      </c>
-      <c r="M11" s="4">
-        <v>1</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="45" t="s">
+      <c r="E11" s="19">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="46">
+        <v>1</v>
+      </c>
+      <c r="L11" s="47">
+        <v>1</v>
+      </c>
+      <c r="M11" s="47">
+        <v>1</v>
+      </c>
+      <c r="N11" s="47">
+        <v>0</v>
+      </c>
+      <c r="O11" s="47">
+        <v>1</v>
+      </c>
+      <c r="P11" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="Q11" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="45"/>
+      <c r="R11" s="48"/>
       <c r="S11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="9">
         <v>59</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="37">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="19">
-        <v>1</v>
-      </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="45"/>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="46"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="48"/>
       <c r="S12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="28">
+      <c r="B13" s="27"/>
+      <c r="C13" s="10">
         <v>60</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="38">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7">
-        <v>1</v>
-      </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="39">
-        <v>0</v>
-      </c>
-      <c r="K13" s="46">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6">
-        <v>1</v>
-      </c>
-      <c r="O13" s="6" t="s">
+      <c r="E13" s="20">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="21">
+        <v>0</v>
+      </c>
+      <c r="K13" s="54">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>1</v>
+      </c>
+      <c r="M13" s="42">
+        <v>1</v>
+      </c>
+      <c r="N13" s="42">
+        <v>1</v>
+      </c>
+      <c r="O13" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="47" t="s">
+      <c r="P13" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="46" t="s">
+      <c r="Q13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="R13" s="47"/>
+      <c r="R13" s="44"/>
     </row>
     <row r="14" spans="1:19" ht="16" thickBot="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="29">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="11">
         <v>64</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="40">
-        <v>1</v>
-      </c>
-      <c r="F14" s="41">
-        <v>1</v>
-      </c>
-      <c r="G14" s="41">
-        <v>1</v>
-      </c>
-      <c r="H14" s="41">
-        <v>1</v>
-      </c>
-      <c r="I14" s="41">
-        <v>1</v>
-      </c>
-      <c r="J14" s="42">
-        <v>1</v>
-      </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="50"/>
+      <c r="E14" s="22">
+        <v>1</v>
+      </c>
+      <c r="F14" s="23">
+        <v>1</v>
+      </c>
+      <c r="G14" s="23">
+        <v>1</v>
+      </c>
+      <c r="H14" s="23">
+        <v>1</v>
+      </c>
+      <c r="I14" s="23">
+        <v>1</v>
+      </c>
+      <c r="J14" s="24">
+        <v>1</v>
+      </c>
+      <c r="K14" s="55"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="Q13:R14"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="R3:R8"/>
+    <mergeCell ref="R10:R12"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="A3:B8"/>
@@ -1773,35 +1810,6 @@
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="R3:R8"/>
-    <mergeCell ref="R10:R12"/>
-    <mergeCell ref="Q13:R14"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>